<commit_message>
Minor bug fixes Changed driver controls Added enable, disable functions to the Subsystems Don't use timer in shooter except in autonomous Freed PID on disable Made Hybrid initialization and calling more efficient
</commit_message>
<xml_diff>
--- a/Ports for Robot.xlsx
+++ b/Ports for Robot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -237,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -259,6 +259,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,7 +595,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.85546875" defaultRowHeight="16"/>
@@ -716,6 +719,7 @@
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="C11" s="10"/>
       <c r="D11" s="9" t="s">
         <v>3</v>
       </c>
@@ -841,7 +845,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.51"/>
-  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;LLast Edited: David Grossman&amp;CFebruary 20, 2012&amp;R FRC Team 811</oddHeader>
   </headerFooter>

</xml_diff>